<commit_message>
Cambios en el doc
Cambios varios
</commit_message>
<xml_diff>
--- a/Proyecto de grado IIND/1. Datos/4. Bogota_Promedio_Dias.xlsx
+++ b/Proyecto de grado IIND/1. Datos/4. Bogota_Promedio_Dias.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\windows\Documents\GitHub\Problem_Set_1\Proyecto-de-grado-IIND\Proyecto de grado IIND\1. Datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D74F598D-5840-444B-B386-B21AA87B692A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79D42671-75F8-4698-A2F2-9611DB1AC894}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -155,6 +155,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>220153</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>160</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A042A85C-7942-47A0-A831-4DD09F49D798}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12277725" y="571500"/>
+          <a:ext cx="7725853" cy="1143160"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -478,16 +527,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S1250"/>
+  <dimension ref="A1:W1250"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="W11" sqref="W11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -546,7 +598,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>44197</v>
       </c>
@@ -601,8 +653,12 @@
       <c r="S2">
         <v>1.5765151515151521</v>
       </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U2">
+        <f>+I2</f>
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>44198</v>
       </c>
@@ -658,7 +714,7 @@
         <v>1.070075757575758</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>44199</v>
       </c>
@@ -714,7 +770,7 @@
         <v>1.385551948051948</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>44200</v>
       </c>
@@ -770,7 +826,7 @@
         <v>1.2824134199134201</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>44201</v>
       </c>
@@ -826,7 +882,7 @@
         <v>1.240530303030303</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>44202</v>
       </c>
@@ -882,7 +938,7 @@
         <v>1.1264646464646459</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>44203</v>
       </c>
@@ -938,7 +994,7 @@
         <v>1.5946969696969699</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>44204</v>
       </c>
@@ -994,7 +1050,7 @@
         <v>1.0075216450216451</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>44205</v>
       </c>
@@ -1050,7 +1106,7 @@
         <v>1.31504329004329</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>44206</v>
       </c>
@@ -1105,8 +1161,19 @@
       <c r="S11">
         <v>1.413888888888889</v>
       </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U11">
+        <v>22</v>
+      </c>
+      <c r="V11">
+        <f>+(I2/10^6)*1000*(1/U12)*(28.01/1)*(10^6/1)</f>
+        <v>351.41014876672205</v>
+      </c>
+      <c r="W11">
+        <f>+I2*1.15</f>
+        <v>0.45999999999999996</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>44207</v>
       </c>
@@ -1161,8 +1228,12 @@
       <c r="S12">
         <v>1.4015151515151509</v>
       </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U12">
+        <f>((0.082*(M2+273.15))/(R2/760))</f>
+        <v>31.882972188824283</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>44208</v>
       </c>
@@ -1218,7 +1289,7 @@
         <v>1.803409090909091</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>44209</v>
       </c>
@@ -1274,7 +1345,7 @@
         <v>1.32405303030303</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>44210</v>
       </c>
@@ -1330,7 +1401,7 @@
         <v>1.261676548089592</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>44211</v>
       </c>
@@ -68646,5 +68717,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>